<commit_message>
updated prompts and fixed edgecase in yes/no
</commit_message>
<xml_diff>
--- a/backend/following_list/following_list.xlsx
+++ b/backend/following_list/following_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielgeorge/Documents/work/ml/small-stuff/twitter-llm-feed/backend/following_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52989BA-B493-E641-A3BA-E7B9447A48AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC4FE6A-462D-CC46-92C2-3CA64CE0036E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{03FDC343-27EF-0740-A5A2-D0CC9CFD1B82}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{03FDC343-27EF-0740-A5A2-D0CC9CFD1B82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>_akhaliq</t>
   </si>
@@ -129,17 +129,31 @@
     <t>- Actual information/realizations/advice you'd think is worth telling me</t>
   </si>
   <si>
+    <t>- Startup advice</t>
+  </si>
+  <si>
+    <t>- AI x Biology/Healthcare 
+- Applications of multimodal transformer models and improvements to them
+    - ex. LLM agent that uses vision to perform tasks on web browsers through screenshots (NOT normal transformer applications)
+- Using LLMs to create new interfaces
+    - ex. turning text into a graph or flow chart
+- Startup launches
+    - Only if they say how much they got funding (ex. Series A)
+- Breakthroughs that are related to projects in my backlogs
+    - AI text games combined with spaced repetition like Zork
+    - Generating out-of-distribution ideas with LLMs
+    - Music Generation</t>
+  </si>
+  <si>
     <t>- Politics, culture, drama, news
     - Basically, things that I have no control over and won't help me
-- AI Safety, Diffusion models
-- Research that is too technical and not DIRECTLY useable to my current work
+- Image creation models (ex. stable diffusion, midjourney, etc)
+    - I am not working on craeting images right now
+- Research that is not DIRECTLY useable to my current work and theoretical
     - ex. novel loss functions, pre-training hacks, large-scale training
-    - there is a lot of machine learning research coming out and most of it isn't useable or relevant to the work I'm doing
+    - Everything akhaliq posts is about AI so that is NOT a good reason in itself for reccomending a post. A lot of the machine learning research coming out isn't useable or relevant to the work I'm doing
 - Time sinks that take me away from my work
     - I get nerd-sniped often, and it's one of the biggest things I need help with. If something doesn't fit the interested criteria, please shield me from getting nerd-sniped.</t>
-  </si>
-  <si>
-    <t>- Startup advice</t>
   </si>
 </sst>
 </file>
@@ -509,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17642FBB-377D-ED4D-A379-4F3B3A1FFA37}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,15 +545,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="238" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -547,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>

</xml_diff>